<commit_message>
Test Data changes - Time Record Manager - 3 July 2024
</commit_message>
<xml_diff>
--- a/TestData/LV_TMTT0009535_VerifyRateGenerationToStaffWithDifferentTitleInSummaryAndDetailsLogTabLightningView.xlsx
+++ b/TestData/LV_TMTT0009535_VerifyRateGenerationToStaffWithDifferentTitleInSummaryAndDetailsLogTabLightningView.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vkumar0427\source\repos\SF_Automation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC04086-6909-49F0-8B7A-18410298A8BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594893B8-FA9C-4548-BD4B-B9A25D435E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="5" r:id="rId1"/>
@@ -152,12 +152,6 @@
     <t>DRC - Original</t>
   </si>
   <si>
-    <t>Rahimeh Bahrampourian</t>
-  </si>
-  <si>
-    <t>Salesforce Administrator</t>
-  </si>
-  <si>
     <t>Ashley Choi</t>
   </si>
   <si>
@@ -186,6 +180,12 @@
   </si>
   <si>
     <t>Time Record Manager</t>
+  </si>
+  <si>
+    <t>Executive Administrator</t>
+  </si>
+  <si>
+    <t>Nicole Bicho</t>
   </si>
 </sst>
 </file>
@@ -523,37 +523,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -570,19 +570,19 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -598,19 +598,19 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -626,17 +626,17 @@
       <selection activeCell="D1" sqref="D1:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="61.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -656,7 +656,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -676,7 +676,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -696,7 +696,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -716,7 +716,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -750,16 +750,16 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="61.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -776,7 +776,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -793,7 +793,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -810,7 +810,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -827,7 +827,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -858,14 +858,14 @@
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="61.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -873,7 +873,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -881,7 +881,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -889,7 +889,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -897,7 +897,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -915,18 +915,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.140625" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -934,21 +934,21 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -959,7 +959,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
@@ -970,7 +970,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
21 Jan 2025 - Final
</commit_message>
<xml_diff>
--- a/TestData/LV_TMTT0009535_VerifyRateGenerationToStaffWithDifferentTitleInSummaryAndDetailsLogTabLightningView.xlsx
+++ b/TestData/LV_TMTT0009535_VerifyRateGenerationToStaffWithDifferentTitleInSummaryAndDetailsLogTabLightningView.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vkumar0427\source\repos\SF_Automation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F26CFFE-6C3B-40B4-A375-4A39097B8DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D23009-60BC-4261-80FC-215E6A06C7DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -524,7 +524,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -916,7 +916,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
26 Feb 2025 - Mid - Time Record
</commit_message>
<xml_diff>
--- a/TestData/LV_TMTT0009535_VerifyRateGenerationToStaffWithDifferentTitleInSummaryAndDetailsLogTabLightningView.xlsx
+++ b/TestData/LV_TMTT0009535_VerifyRateGenerationToStaffWithDifferentTitleInSummaryAndDetailsLogTabLightningView.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D23009-60BC-4261-80FC-215E6A06C7DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF964D3-1CE4-4692-96CC-A8AB88B08D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="5" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="46">
   <si>
     <t>Global Search User</t>
   </si>
@@ -137,18 +137,6 @@
     <t>0</t>
   </si>
   <si>
-    <t>(MEH) Thompson_CLP Toxicology-Thompson Hine, LLP-FVA-26495</t>
-  </si>
-  <si>
-    <t>Debevoise_Xie (Consulting)-Debevoise &amp; Plimpton LLP-FVA-26378</t>
-  </si>
-  <si>
-    <t>(GB) Anthony_ACOVA-Anthony Ostlund Baer &amp; Louwagie P.A.-FVA-27471</t>
-  </si>
-  <si>
-    <t>Eventide-Eventide Asset Management, LLC-FVA-111771</t>
-  </si>
-  <si>
     <t>DRC - Original</t>
   </si>
   <si>
@@ -186,13 +174,19 @@
   </si>
   <si>
     <t>Executive Administrator</t>
+  </si>
+  <si>
+    <t>Project Agility - 87746</t>
+  </si>
+  <si>
+    <t>CF-87746</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,6 +205,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -539,21 +539,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
         <v>36</v>
-      </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -577,12 +577,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -594,7 +594,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81CF81A0-141C-44BF-BC82-4486379D0B0F}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -605,12 +605,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -622,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -657,8 +657,8 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>31</v>
+      <c r="A2" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>13</v>
@@ -677,8 +677,8 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>32</v>
+      <c r="A3" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>13</v>
@@ -697,8 +697,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>33</v>
+      <c r="A4" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>13</v>
@@ -717,8 +717,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>34</v>
+      <c r="A5" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>13</v>
@@ -737,6 +737,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -747,7 +748,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -777,8 +778,8 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>31</v>
+      <c r="A2" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>14</v>
@@ -794,8 +795,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>32</v>
+      <c r="A3" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>14</v>
@@ -811,8 +812,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>33</v>
+      <c r="A4" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>14</v>
@@ -828,8 +829,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>34</v>
+      <c r="A5" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>14</v>
@@ -855,7 +856,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -875,34 +876,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
         <v>31</v>
-      </c>
-      <c r="B2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -915,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -934,15 +935,15 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>

</xml_diff>